<commit_message>
28,11,2024 wykres nierówno brak obiektu session action niby działa ale nie user data - wiele kolumn niż nazw nie zawija się po add_variable
</commit_message>
<xml_diff>
--- a/datasets/rna-seq szblon — kopia.xlsx
+++ b/datasets/rna-seq szblon — kopia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projekt_mgr\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F4881E-EDFC-4AB4-AF8E-14A143D332AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5708926C-E5C1-4BA8-BE68-19916BA02CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14430" yWindow="0" windowWidth="14370" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>gene</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
     <t>logFC</t>
   </si>
   <si>
@@ -48,9 +42,6 @@
     <t>add.variable</t>
   </si>
   <si>
-    <t>strand</t>
-  </si>
-  <si>
     <t>SCO1550</t>
   </si>
   <si>
@@ -58,9 +49,6 @@
   </si>
   <si>
     <t>SCO2166</t>
-  </si>
-  <si>
-    <t>width</t>
   </si>
 </sst>
 </file>
@@ -429,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +428,7 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,102 +439,90 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4.4999999999999999E-18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-14.1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2E-14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="G2" s="3">
-        <v>4.4999999999999999E-18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>-14.1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>2E-14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="B4" s="1">
         <v>-10.8</v>
       </c>
-      <c r="G4" s="3">
+      <c r="C4" s="3">
         <v>1.7E-16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F5" s="1"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F8" s="1"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F9" s="1"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" s="2"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16" s="1"/>
       <c r="G16" s="4"/>
     </row>

</xml_diff>